<commit_message>
14010802 new from mohandes
</commit_message>
<xml_diff>
--- a/DoctorFAM.Presentation/wwwroot/Content/ExcelSampleFile/PopulationCoveredSmple.xlsx
+++ b/DoctorFAM.Presentation/wwwroot/Content/ExcelSampleFile/PopulationCoveredSmple.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ParsaPanahpoor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DoctorFAM\DoctorFAM.Presentation\wwwroot\Content\ExcelSampleFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF8B414-4C3B-4EBD-92BC-9A8FA977DF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FCFC96-3898-4BD3-BB99-AEB38CDEABDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3BCE8929-E281-41EA-BFEF-04CA297337B1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{3BCE8929-E281-41EA-BFEF-04CA297337B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -174,6 +174,7 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,18 +492,18 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -511,7 +512,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,5 +531,6 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>